<commit_message>
Update file di test con campi opzionali
Update file CDA di test con campi opzionali per RAD e LDO
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-RAD/3.24.0.0/accreditamento-checklist_V8.2.6.xlsx
+++ b/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-RAD/3.24.0.0/accreditamento-checklist_V8.2.6.xlsx
@@ -745,13 +745,13 @@
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-08-07T07:13:36:00Z</t>
-  </si>
-  <si>
-    <t>7d72321e94a0f14f763842828faeb3dc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.ef9b9c4d23e560db876fa7c5866c0bf73ac57069a2bd3e8d00e77c2ccaf1a515.0d03254e58^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-08-26T08:54:22:00Z</t>
+  </si>
+  <si>
+    <t>b12a33c9fe173515abfdfb8223b2f747</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.ef9b9c4d23e560db876fa7c5866c0bf73ac57069a2bd3e8d00e77c2ccaf1a515.3d6013f551^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>OK</t>
@@ -795,13 +795,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-08-07T07:04:42:00Z</t>
-  </si>
-  <si>
-    <t>f018c65904676c62b1c2dd6855877245</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.82a1bcb3ceea777f60fd153f6ec968824d48cbdd877242dfde81a97ed7d9e51f.4717be86b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-08-26T08:57:54:00Z</t>
+  </si>
+  <si>
+    <t>40764cb737f6dd3adba2c378649c2a7e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.82a1bcb3ceea777f60fd153f6ec968824d48cbdd877242dfde81a97ed7d9e51f.42a9e275ce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT26</t>
@@ -5422,7 +5422,7 @@
         <v>170</v>
       </c>
       <c r="F53" s="36">
-        <v>45876</v>
+        <v>45895</v>
       </c>
       <c r="G53" s="36" t="s">
         <v>171</v>
@@ -5633,7 +5633,7 @@
         <v>185</v>
       </c>
       <c r="F58" s="41">
-        <v>45876</v>
+        <v>45895</v>
       </c>
       <c r="G58" s="36" t="s">
         <v>186</v>

</xml_diff>

<commit_message>
Update file per accreditamento dopo test automatici
Update file per accreditamento dopo test automatici
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-RAD/3.24.0.0/accreditamento-checklist_V8.2.6.xlsx
+++ b/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-RAD/3.24.0.0/accreditamento-checklist_V8.2.6.xlsx
@@ -745,13 +745,13 @@
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-08-26T08:54:22:00Z</t>
-  </si>
-  <si>
-    <t>b12a33c9fe173515abfdfb8223b2f747</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.ef9b9c4d23e560db876fa7c5866c0bf73ac57069a2bd3e8d00e77c2ccaf1a515.3d6013f551^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-08-27T08:15:45:00Z</t>
+  </si>
+  <si>
+    <t>32664e6a3b0a75a047d98d2239b67932</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.ef9b9c4d23e560db876fa7c5866c0bf73ac57069a2bd3e8d00e77c2ccaf1a515.96c061303b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>OK</t>
@@ -795,13 +795,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-08-26T08:57:54:00Z</t>
-  </si>
-  <si>
-    <t>40764cb737f6dd3adba2c378649c2a7e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.82a1bcb3ceea777f60fd153f6ec968824d48cbdd877242dfde81a97ed7d9e51f.42a9e275ce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-08-27T08:13:06:00Z</t>
+  </si>
+  <si>
+    <t>13bb96e6ac69eee4e5991972646fe636</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.82a1bcb3ceea777f60fd153f6ec968824d48cbdd877242dfde81a97ed7d9e51f.e4795b1398^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT26</t>
@@ -5422,7 +5422,7 @@
         <v>170</v>
       </c>
       <c r="F53" s="36">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="G53" s="36" t="s">
         <v>171</v>
@@ -5633,7 +5633,7 @@
         <v>185</v>
       </c>
       <c r="F58" s="41">
-        <v>45895</v>
+        <v>45896</v>
       </c>
       <c r="G58" s="36" t="s">
         <v>186</v>

</xml_diff>

<commit_message>
Update test 448 RSA
Update del campo ClinicalDocument/component/structuredBody/component/section[ID=Storia_Clinica]/component/section[ID=Allergie]/title
per test 448 RSA
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-RAD/3.24.0.0/accreditamento-checklist_V8.2.6.xlsx
+++ b/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-RAD/3.24.0.0/accreditamento-checklist_V8.2.6.xlsx
@@ -745,13 +745,13 @@
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-08-27T08:15:45:00Z</t>
-  </si>
-  <si>
-    <t>32664e6a3b0a75a047d98d2239b67932</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.ef9b9c4d23e560db876fa7c5866c0bf73ac57069a2bd3e8d00e77c2ccaf1a515.96c061303b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-09-03T07:12:12:00Z</t>
+  </si>
+  <si>
+    <t>6896c74cab395a45f4b620a535a4c5fa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.ef9b9c4d23e560db876fa7c5866c0bf73ac57069a2bd3e8d00e77c2ccaf1a515.e39a698380^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>OK</t>
@@ -5422,7 +5422,7 @@
         <v>170</v>
       </c>
       <c r="F53" s="36">
-        <v>45896</v>
+        <v>45903</v>
       </c>
       <c r="G53" s="36" t="s">
         <v>171</v>

</xml_diff>